<commit_message>
atualizei as tabelas de teste e fiz teste da classe viagem
</commit_message>
<xml_diff>
--- a/tabelaUnitaria.xlsx
+++ b/tabelaUnitaria.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csf14\Desktop\trabalhoVVFinal\Veifica-oeValida-oSoftware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2604E96-CBF3-457A-9A46-D09693B43D2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F033FB-2443-456C-809F-E43E797F1D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{380BA23A-B45B-486C-9841-AE19EE764F2C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{380BA23A-B45B-486C-9841-AE19EE764F2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="1" r:id="rId1"/>
     <sheet name="Bairro" sheetId="2" r:id="rId2"/>
+    <sheet name="Viagem" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>pontoCentral()</t>
   </si>
@@ -166,6 +167,87 @@
   </si>
   <si>
     <t>novoBairroQuadrado()</t>
+  </si>
+  <si>
+    <t>casos de teste</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>teste novoBairroQuadrado1()</t>
+  </si>
+  <si>
+    <t>nome="Chacara das Pedras", ponto (10,5), lado=3, custo da Viagem= 0.05</t>
+  </si>
+  <si>
+    <t>ponto Inferior Direito com a coordenada (13,2)</t>
+  </si>
+  <si>
+    <t>teste novoBairroRetangular1()</t>
+  </si>
+  <si>
+    <t>nome="Chacara das Pedras", ponto (10,5), ladoH=8, ladoV= 3, custo da Viagem= 0.05</t>
+  </si>
+  <si>
+    <t>ponto Inferior Direito com a coordenada (18,2)</t>
+  </si>
+  <si>
+    <t>nome="Chacara das Pedras", ponto (10,5), lado=3, custo da Viagem= -0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar mensagem de exceção </t>
+  </si>
+  <si>
+    <t>nome="Chacara das Pedras", ponto (10,5), ladoH=8, ladoV= 3, custo da Viagem= -5.09</t>
+  </si>
+  <si>
+    <t>novoBairroRetangular()</t>
+  </si>
+  <si>
+    <t>teste novoBairroRetangular2()</t>
+  </si>
+  <si>
+    <t>teste novoBairroQuadrado()</t>
+  </si>
+  <si>
+    <t>AlterarCustoTransporte</t>
+  </si>
+  <si>
+    <t>teste alterarCustoTransporte1()</t>
+  </si>
+  <si>
+    <t>nome="Chacara das Pedras", ponto (10,5), lado=3, custo do transporte= 0.05, alterar custo do transporte para 1.25</t>
+  </si>
+  <si>
+    <t>getCustoTransporte devolve 1.25</t>
+  </si>
+  <si>
+    <t>teste alterarCustoTransporte2()</t>
+  </si>
+  <si>
+    <t>devolve mensagem de exceção</t>
+  </si>
+  <si>
+    <t>nome="Chacara das Pedras", ponto (10,5), lado=3, custo do transporte= 0.05, alterar custo do transporte para -0.35</t>
+  </si>
+  <si>
+    <t>Teste da classe</t>
+  </si>
+  <si>
+    <t>teste construtor1</t>
+  </si>
+  <si>
+    <t>Viagem com valorCobrado=-50</t>
+  </si>
+  <si>
+    <t>teste dataHora</t>
+  </si>
+  <si>
+    <t>dataHora com mês=22</t>
+  </si>
+  <si>
+    <t>mostrar mensagem de exceção</t>
   </si>
 </sst>
 </file>
@@ -202,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -225,15 +307,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,10 +370,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -571,86 +706,86 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="3" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="K3" s="4" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="T3" s="4" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="T3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="K4" s="4" t="s">
+      <c r="H4" s="3"/>
+      <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="2" t="s">
+      <c r="L4" s="2"/>
+      <c r="M4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="4" t="s">
+      <c r="N4" s="3"/>
+      <c r="O4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="2" t="s">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="T4" s="4" t="s">
+      <c r="R4" s="3"/>
+      <c r="T4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="4"/>
-      <c r="V4" s="2" t="s">
+      <c r="U4" s="2"/>
+      <c r="V4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="W4" s="2"/>
-      <c r="X4" s="4" t="s">
+      <c r="W4" s="3"/>
+      <c r="X4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="2" t="s">
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AA4" s="2"/>
+      <c r="AA4" s="3"/>
     </row>
     <row r="5" spans="1:27" ht="174" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -665,8 +800,8 @@
         <v>28</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
       <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
@@ -703,8 +838,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
       <c r="K6" s="1" t="s">
         <v>13</v>
       </c>
@@ -741,8 +876,8 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -767,8 +902,8 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -793,8 +928,8 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -819,8 +954,8 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -845,8 +980,8 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -871,8 +1006,8 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -891,10 +1026,10 @@
       <c r="AA12" s="1"/>
     </row>
     <row r="13" spans="1:27" ht="174" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
@@ -903,8 +1038,8 @@
         <v>31</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -943,8 +1078,8 @@
         <v>42</v>
       </c>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K15" s="1"/>
@@ -961,8 +1096,8 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K16" s="1"/>
@@ -979,8 +1114,8 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K17" s="1" t="s">
@@ -1003,8 +1138,8 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K18" s="1"/>
@@ -1021,8 +1156,8 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K19" s="1"/>
@@ -1039,8 +1174,8 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K20" s="1"/>
@@ -1057,8 +1192,8 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K21" s="1"/>
@@ -1075,8 +1210,8 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K22" s="1"/>
@@ -1093,8 +1228,8 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K23" s="1"/>
@@ -1111,8 +1246,8 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K24" s="1"/>
@@ -1129,8 +1264,8 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K25" s="1"/>
@@ -1143,16 +1278,16 @@
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1163,22 +1298,22 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="4" t="s">
+      <c r="D27" s="3"/>
+      <c r="E27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="2" t="s">
+      <c r="F27" s="2"/>
+      <c r="G27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="3"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1552,11 +1687,52 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="G44:H51"/>
-    <mergeCell ref="C5:D12"/>
-    <mergeCell ref="E5:F12"/>
-    <mergeCell ref="G5:H12"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="V6:W13"/>
+    <mergeCell ref="X6:Y13"/>
+    <mergeCell ref="Z6:AA13"/>
+    <mergeCell ref="T6:U13"/>
+    <mergeCell ref="T14:U24"/>
+    <mergeCell ref="V14:W24"/>
+    <mergeCell ref="X14:Y24"/>
+    <mergeCell ref="Z14:AA24"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="T3:AA3"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="O29:P39"/>
+    <mergeCell ref="Q29:R39"/>
+    <mergeCell ref="O6:P16"/>
+    <mergeCell ref="Q6:R16"/>
+    <mergeCell ref="K17:L28"/>
+    <mergeCell ref="M17:N28"/>
+    <mergeCell ref="O17:P28"/>
+    <mergeCell ref="Q17:R28"/>
+    <mergeCell ref="M6:N16"/>
+    <mergeCell ref="K6:L16"/>
+    <mergeCell ref="K29:L39"/>
+    <mergeCell ref="M29:N39"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="A44:B51"/>
     <mergeCell ref="C44:D51"/>
     <mergeCell ref="E44:F51"/>
@@ -1570,54 +1746,13 @@
     <mergeCell ref="A36:B43"/>
     <mergeCell ref="C36:D43"/>
     <mergeCell ref="E36:F43"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="O29:P39"/>
-    <mergeCell ref="Q29:R39"/>
-    <mergeCell ref="O6:P16"/>
-    <mergeCell ref="Q6:R16"/>
-    <mergeCell ref="K17:L28"/>
-    <mergeCell ref="M17:N28"/>
-    <mergeCell ref="O17:P28"/>
-    <mergeCell ref="Q17:R28"/>
-    <mergeCell ref="M6:N16"/>
-    <mergeCell ref="K6:L16"/>
-    <mergeCell ref="K29:L39"/>
-    <mergeCell ref="M29:N39"/>
-    <mergeCell ref="T3:AA3"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="V6:W13"/>
-    <mergeCell ref="X6:Y13"/>
-    <mergeCell ref="Z6:AA13"/>
-    <mergeCell ref="T6:U13"/>
-    <mergeCell ref="T14:U24"/>
-    <mergeCell ref="V14:W24"/>
-    <mergeCell ref="X14:Y24"/>
-    <mergeCell ref="Z14:AA24"/>
+    <mergeCell ref="G44:H51"/>
+    <mergeCell ref="C5:D12"/>
+    <mergeCell ref="E5:F12"/>
+    <mergeCell ref="G5:H12"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="G36:H43"/>
     <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G28:H35"/>
   </mergeCells>
@@ -1627,29 +1762,441 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B83307-777D-4A3B-B190-69081518A722}">
-  <dimension ref="B2:I2"/>
+  <dimension ref="B2:S21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="2:19" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="2:19" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="2:19" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="L6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="2:19" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="2:19" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="B13:C21"/>
+    <mergeCell ref="D13:E21"/>
+    <mergeCell ref="F13:G21"/>
+    <mergeCell ref="H13:I21"/>
+    <mergeCell ref="L3:S3"/>
+    <mergeCell ref="H5:I6"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="D9:E12"/>
+    <mergeCell ref="B9:C12"/>
+    <mergeCell ref="F9:G12"/>
+    <mergeCell ref="H9:I12"/>
+    <mergeCell ref="R6:S7"/>
+    <mergeCell ref="N6:O7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="P6:Q7"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="L4:M5"/>
+    <mergeCell ref="P4:Q5"/>
+    <mergeCell ref="R4:S5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE477CB4-D38C-4B3D-8EEF-AF8A6805173C}">
+  <dimension ref="B2:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="B2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="2:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="13">
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="F4:G5"/>
+    <mergeCell ref="H4:I5"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="H6:I7"/>
     <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
todos testes unitarios estão realizados em entidades, além do teste de integração do roteiro rodando corretamente
</commit_message>
<xml_diff>
--- a/tabelaUnitaria.xlsx
+++ b/tabelaUnitaria.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csf14\Desktop\trabalhoVVFinal\Veifica-oeValida-oSoftware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F033FB-2443-456C-809F-E43E797F1D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3C45A8-AA34-4D48-ADCD-B34086E79F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{380BA23A-B45B-486C-9841-AE19EE764F2C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{380BA23A-B45B-486C-9841-AE19EE764F2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="1" r:id="rId1"/>
     <sheet name="Bairro" sheetId="2" r:id="rId2"/>
     <sheet name="Viagem" sheetId="3" r:id="rId3"/>
+    <sheet name="Passageiro" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
   <si>
     <t>pontoCentral()</t>
   </si>
@@ -248,6 +249,48 @@
   </si>
   <si>
     <t>mostrar mensagem de exceção</t>
+  </si>
+  <si>
+    <t>passageiroExistente()</t>
+  </si>
+  <si>
+    <t>teste passageiroExistente1</t>
+  </si>
+  <si>
+    <t>Passageiro com cpf=1234567, nome= Arthur Morgan, pontuacaoAcumulada= -50 e qtdadeAvaliacoes=5</t>
+  </si>
+  <si>
+    <t>teste passageiroExistente2</t>
+  </si>
+  <si>
+    <t>Passageiro com cpf=1234567, nome= Arthur Morgan, pontuacaoAcumulada= 16 e qtdadeAvaliacoes=-5</t>
+  </si>
+  <si>
+    <t>getPontuacaoMedia()</t>
+  </si>
+  <si>
+    <t>teste getPontuacaoMedia1</t>
+  </si>
+  <si>
+    <t>Passageiro com cpf=1234567, nome= Arthur Morgan, pontuacaoAcumulada= 33 e qtdadeAvaliacoes=5</t>
+  </si>
+  <si>
+    <t>getPontuacaoMedia devolve 6</t>
+  </si>
+  <si>
+    <t>infoPontuacao()</t>
+  </si>
+  <si>
+    <t>teste infoPontuacao1</t>
+  </si>
+  <si>
+    <t>novo passageiro com cpf=1234567, nome= Arthur Morgan, recebe uma pontucao=-5</t>
+  </si>
+  <si>
+    <t>novo passageiro com cpf=1234567, nome= Arthur Morgan, recebe uma pontucao=7</t>
+  </si>
+  <si>
+    <t>pontuacaoAcumulado devolve 15 e qtdAvaliacoes devolve 2</t>
   </si>
 </sst>
 </file>
@@ -362,10 +405,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -706,86 +749,86 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="3" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="K3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="K3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="T3" s="2" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="T3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
     </row>
     <row r="4" spans="1:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="K4" s="2" t="s">
+      <c r="H4" s="2"/>
+      <c r="K4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3" t="s">
+      <c r="L4" s="3"/>
+      <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="2" t="s">
+      <c r="N4" s="2"/>
+      <c r="O4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="3" t="s">
+      <c r="P4" s="3"/>
+      <c r="Q4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="3"/>
-      <c r="T4" s="2" t="s">
+      <c r="R4" s="2"/>
+      <c r="T4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="3" t="s">
+      <c r="U4" s="3"/>
+      <c r="V4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W4" s="3"/>
-      <c r="X4" s="2" t="s">
+      <c r="W4" s="2"/>
+      <c r="X4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="3" t="s">
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AA4" s="3"/>
+      <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="174" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -800,8 +843,8 @@
         <v>28</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
@@ -838,8 +881,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="K6" s="1" t="s">
         <v>13</v>
       </c>
@@ -876,8 +919,8 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -902,8 +945,8 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -928,8 +971,8 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -954,8 +997,8 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -980,8 +1023,8 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1006,8 +1049,8 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1038,8 +1081,8 @@
         <v>31</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1078,8 +1121,8 @@
         <v>42</v>
       </c>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K15" s="1"/>
@@ -1096,8 +1139,8 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K16" s="1"/>
@@ -1114,8 +1157,8 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K17" s="1" t="s">
@@ -1138,8 +1181,8 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K18" s="1"/>
@@ -1156,8 +1199,8 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K19" s="1"/>
@@ -1174,8 +1217,8 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K20" s="1"/>
@@ -1192,8 +1235,8 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K21" s="1"/>
@@ -1210,8 +1253,8 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="2"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K22" s="1"/>
@@ -1228,8 +1271,8 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="2"/>
-      <c r="AA22" s="2"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K23" s="1"/>
@@ -1246,8 +1289,8 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
-      <c r="Z23" s="2"/>
-      <c r="AA23" s="2"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K24" s="1"/>
@@ -1264,8 +1307,8 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
-      <c r="Z24" s="2"/>
-      <c r="AA24" s="2"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K25" s="1"/>
@@ -1278,16 +1321,16 @@
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1298,22 +1341,22 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="3" t="s">
+      <c r="F27" s="3"/>
+      <c r="G27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="3"/>
+      <c r="H27" s="2"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1687,6 +1730,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="G44:H51"/>
+    <mergeCell ref="C5:D12"/>
+    <mergeCell ref="E5:F12"/>
+    <mergeCell ref="G5:H12"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="G36:H43"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G28:H35"/>
+    <mergeCell ref="A44:B51"/>
+    <mergeCell ref="C44:D51"/>
+    <mergeCell ref="E44:F51"/>
+    <mergeCell ref="A5:B12"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A28:B35"/>
+    <mergeCell ref="C28:D35"/>
+    <mergeCell ref="E28:F35"/>
+    <mergeCell ref="A36:B43"/>
+    <mergeCell ref="C36:D43"/>
+    <mergeCell ref="E36:F43"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="O29:P39"/>
+    <mergeCell ref="Q29:R39"/>
+    <mergeCell ref="O6:P16"/>
+    <mergeCell ref="Q6:R16"/>
+    <mergeCell ref="K17:L28"/>
+    <mergeCell ref="M17:N28"/>
+    <mergeCell ref="O17:P28"/>
+    <mergeCell ref="Q17:R28"/>
+    <mergeCell ref="M6:N16"/>
+    <mergeCell ref="K6:L16"/>
+    <mergeCell ref="K29:L39"/>
+    <mergeCell ref="M29:N39"/>
+    <mergeCell ref="T3:AA3"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="X5:Y5"/>
@@ -1703,58 +1798,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="T3:AA3"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="O29:P39"/>
-    <mergeCell ref="Q29:R39"/>
-    <mergeCell ref="O6:P16"/>
-    <mergeCell ref="Q6:R16"/>
-    <mergeCell ref="K17:L28"/>
-    <mergeCell ref="M17:N28"/>
-    <mergeCell ref="O17:P28"/>
-    <mergeCell ref="Q17:R28"/>
-    <mergeCell ref="M6:N16"/>
-    <mergeCell ref="K6:L16"/>
-    <mergeCell ref="K29:L39"/>
-    <mergeCell ref="M29:N39"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="A44:B51"/>
-    <mergeCell ref="C44:D51"/>
-    <mergeCell ref="E44:F51"/>
-    <mergeCell ref="A5:B12"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A28:B35"/>
-    <mergeCell ref="C28:D35"/>
-    <mergeCell ref="E28:F35"/>
-    <mergeCell ref="A36:B43"/>
-    <mergeCell ref="C36:D43"/>
-    <mergeCell ref="E36:F43"/>
-    <mergeCell ref="G44:H51"/>
-    <mergeCell ref="C5:D12"/>
-    <mergeCell ref="E5:F12"/>
-    <mergeCell ref="G5:H12"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="G36:H43"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G28:H35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1783,10 +1826,10 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="2:19" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
@@ -1885,8 +1928,8 @@
         <v>53</v>
       </c>
       <c r="Q6" s="1"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
     </row>
     <row r="7" spans="2:19" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L7" s="1"/>
@@ -1895,8 +1938,8 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
@@ -2054,6 +2097,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="L4:M5"/>
+    <mergeCell ref="P4:Q5"/>
+    <mergeCell ref="R4:S5"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="B13:C21"/>
     <mergeCell ref="D13:E21"/>
     <mergeCell ref="F13:G21"/>
@@ -2070,21 +2128,6 @@
     <mergeCell ref="L6:M7"/>
     <mergeCell ref="P6:Q7"/>
     <mergeCell ref="D5:E6"/>
-    <mergeCell ref="B5:C6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="L4:M5"/>
-    <mergeCell ref="P4:Q5"/>
-    <mergeCell ref="R4:S5"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2094,7 +2137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE477CB4-D38C-4B3D-8EEF-AF8A6805173C}">
   <dimension ref="B2:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -2143,8 +2186,8 @@
         <v>70</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
@@ -2153,8 +2196,8 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
@@ -2184,6 +2227,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="D4:E5"/>
     <mergeCell ref="F4:G5"/>
     <mergeCell ref="H4:I5"/>
@@ -2191,13 +2239,398 @@
     <mergeCell ref="D6:E7"/>
     <mergeCell ref="F6:G7"/>
     <mergeCell ref="H6:I7"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="B4:C5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04618F09-DEDC-4672-845A-6EBE5EF7E542}">
+  <dimension ref="D2:V22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15:T22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="O2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="4:22" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="O3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+    </row>
+    <row r="4" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+    </row>
+    <row r="5" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+    </row>
+    <row r="8" spans="4:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="O9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+    </row>
+    <row r="10" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="O10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+    </row>
+    <row r="11" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+    </row>
+    <row r="12" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+    </row>
+    <row r="13" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+    </row>
+    <row r="14" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+    </row>
+    <row r="15" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="O15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="4:22" x14ac:dyDescent="0.35">
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="15:22" x14ac:dyDescent="0.35">
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="15:22" x14ac:dyDescent="0.35">
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="15:22" x14ac:dyDescent="0.35">
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="15:22" x14ac:dyDescent="0.35">
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="15:22" x14ac:dyDescent="0.35">
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="15:22" x14ac:dyDescent="0.35">
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="O9:V9"/>
+    <mergeCell ref="O10:P14"/>
+    <mergeCell ref="Q10:R14"/>
+    <mergeCell ref="S10:T14"/>
+    <mergeCell ref="U10:V14"/>
+    <mergeCell ref="O15:P22"/>
+    <mergeCell ref="Q15:R22"/>
+    <mergeCell ref="S15:T22"/>
+    <mergeCell ref="U15:V22"/>
+    <mergeCell ref="O2:V2"/>
+    <mergeCell ref="O3:P7"/>
+    <mergeCell ref="Q3:R7"/>
+    <mergeCell ref="S3:T7"/>
+    <mergeCell ref="U3:V7"/>
+    <mergeCell ref="F8:G15"/>
+    <mergeCell ref="D8:E15"/>
+    <mergeCell ref="H8:I15"/>
+    <mergeCell ref="J8:K15"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="F3:G7"/>
+    <mergeCell ref="D3:E7"/>
+    <mergeCell ref="H3:I7"/>
+    <mergeCell ref="J3:K7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>